<commit_message>
YAML의 key를 통해 req data encrypt
</commit_message>
<xml_diff>
--- a/펌뱅킹-테이블설계.xlsx
+++ b/펌뱅킹-테이블설계.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judyi\Desktop\class\inspien\Firmbanking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF094C4-3308-43CC-A837-1F97ADAFED03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7917C4CA-C0C0-40B9-B5CB-B41D0D7FB922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{478546EF-A667-4BE7-9398-D997D40A68D3}"/>
+    <workbookView xWindow="14016" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{478546EF-A667-4BE7-9398-D997D40A68D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
   <si>
     <t>CustMst</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -354,10 +353,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">//상태… 완료/실패!  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>//실제 데이터</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -367,6 +362,34 @@
   </si>
   <si>
     <t>고객별 TelegramNo 관리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">//상태 코드  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TxIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrCode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ErrMsg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NatvTrNo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>//거래 고유 번호 ==&gt; 성공시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -734,13 +757,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D1E0A77-5F01-4F2D-A165-3604F367502A}">
-  <dimension ref="B1:L46"/>
+  <dimension ref="B1:L50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" ySplit="3" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J40" sqref="J40"/>
+      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1120,7 +1143,7 @@
         <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -1197,16 +1220,7 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>2</v>
-      </c>
-      <c r="F29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" t="s">
-        <v>22</v>
-      </c>
-      <c r="K29" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.4">
@@ -1214,16 +1228,16 @@
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="H30" t="s">
         <v>22</v>
       </c>
       <c r="K30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.4">
@@ -1231,16 +1245,16 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="H31" t="s">
         <v>22</v>
       </c>
       <c r="K31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.4">
@@ -1248,16 +1262,16 @@
         <v>4</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F32" t="s">
         <v>15</v>
       </c>
-      <c r="I32" t="s">
+      <c r="H32" t="s">
         <v>22</v>
       </c>
       <c r="K32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.4">
@@ -1265,7 +1279,7 @@
         <v>5</v>
       </c>
       <c r="E33" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F33" t="s">
         <v>15</v>
@@ -1274,7 +1288,7 @@
         <v>22</v>
       </c>
       <c r="K33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.4">
@@ -1282,16 +1296,16 @@
         <v>6</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F34" t="s">
-        <v>56</v>
-      </c>
-      <c r="J34" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="I34" t="s">
+        <v>22</v>
       </c>
       <c r="K34" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.4">
@@ -1299,19 +1313,16 @@
         <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F35" t="s">
-        <v>57</v>
-      </c>
-      <c r="G35" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K35" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.4">
@@ -1319,16 +1330,19 @@
         <v>8</v>
       </c>
       <c r="E36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F36" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+      <c r="G36" t="s">
+        <v>58</v>
       </c>
       <c r="J36" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="K36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.4">
@@ -1336,19 +1350,16 @@
         <v>9</v>
       </c>
       <c r="E37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37">
-        <v>1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>22</v>
+        <v>59</v>
+      </c>
+      <c r="J37" t="s">
+        <v>62</v>
       </c>
       <c r="K37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.4">
@@ -1356,10 +1367,19 @@
         <v>10</v>
       </c>
       <c r="E38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F38" t="s">
-        <v>53</v>
+        <v>15</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
+      <c r="K38" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.4">
@@ -1367,7 +1387,7 @@
         <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F39" t="s">
         <v>53</v>
@@ -1378,119 +1398,167 @@
         <v>12</v>
       </c>
       <c r="E40" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="D41">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
         <v>41</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>55</v>
       </c>
-      <c r="J40" t="s">
+      <c r="J41" t="s">
         <v>64</v>
       </c>
-      <c r="L40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.4">
-      <c r="B41" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41">
-        <v>1</v>
-      </c>
-      <c r="E41" t="s">
-        <v>2</v>
-      </c>
-      <c r="F41" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41">
-        <v>10</v>
-      </c>
-      <c r="H41" t="s">
-        <v>22</v>
+      <c r="L41" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D42">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E42" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
       <c r="F42" t="s">
-        <v>54</v>
-      </c>
-      <c r="H42" t="s">
-        <v>22</v>
+        <v>85</v>
+      </c>
+      <c r="K42" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D43">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E43" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="F43" t="s">
         <v>15</v>
-      </c>
-      <c r="H43" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D44">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E44" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
       <c r="F44" t="s">
-        <v>15</v>
-      </c>
-      <c r="H44" t="s">
-        <v>22</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45" t="s">
+        <v>47</v>
+      </c>
       <c r="D45">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>56</v>
-      </c>
-      <c r="I45" t="s">
-        <v>22</v>
-      </c>
-      <c r="J45" t="s">
-        <v>63</v>
+        <v>15</v>
+      </c>
+      <c r="G45">
+        <v>10</v>
+      </c>
+      <c r="H45" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.4">
       <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F47" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.4">
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" t="s">
+        <v>15</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D49">
+        <v>5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F49" t="s">
+        <v>56</v>
+      </c>
+      <c r="I49" t="s">
+        <v>22</v>
+      </c>
+      <c r="J49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.4">
+      <c r="D50">
         <v>6</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E50" t="s">
         <v>43</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F50" t="s">
         <v>60</v>
       </c>
-      <c r="I46" t="s">
-        <v>22</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="I50" t="s">
+        <v>22</v>
+      </c>
+      <c r="J50" t="s">
         <v>61</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add transfer file logs
</commit_message>
<xml_diff>
--- a/펌뱅킹-테이블설계.xlsx
+++ b/펌뱅킹-테이블설계.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\judyi\Desktop\class\inspien\Firmbanking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7917C4CA-C0C0-40B9-B5CB-B41D0D7FB922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0978B756-F3F9-43E7-ADB4-39CF518FCF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14016" yWindow="17172" windowWidth="23256" windowHeight="12576" xr2:uid="{478546EF-A667-4BE7-9398-D997D40A68D3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{478546EF-A667-4BE7-9398-D997D40A68D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
   <si>
     <t>CustMst</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -760,10 +760,10 @@
   <dimension ref="B1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="3" topLeftCell="F28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="3" topLeftCell="F11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J41" sqref="J41"/>
+      <selection pane="bottomRight" activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>

</xml_diff>